<commit_message>
Edited bash file to describe what's going on a bit more for eLife revisions
</commit_message>
<xml_diff>
--- a/USA/state/output/data_summary/Breakdown of deaths eLife.xlsx
+++ b/USA/state/output/data_summary/Breakdown of deaths eLife.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/mortality/USA/state/output/data_summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-12120" yWindow="-19540" windowWidth="24280" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All ages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="32">
   <si>
     <t>All cause</t>
   </si>
@@ -116,6 +116,15 @@
   <si>
     <t>75 to 84</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Neuropsychiatric disorders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
 </sst>
 </file>
 
@@ -138,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -206,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -226,11 +241,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -241,10 +264,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -254,15 +279,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,137 +563,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="F1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="8">
+        <v>43558203</v>
+      </c>
+      <c r="E2" s="8">
+        <v>42295973</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2+E2</f>
+        <v>85854176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="8">
+        <v>10481582</v>
+      </c>
+      <c r="E3" s="8">
+        <v>9476530</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F18" si="0">D3+E3</f>
+        <v>19958112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="13"/>
+      <c r="D4" s="8">
+        <v>20168049</v>
+      </c>
+      <c r="E4" s="8">
+        <v>21109525</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>41277574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="8">
+        <v>16238344</v>
+      </c>
+      <c r="E5" s="8">
+        <v>17210556</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>33448900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="8">
+        <v>2791652</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2595950</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>5387602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="8">
+        <v>1138053</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1303019</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>2441072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="14"/>
+      <c r="D8" s="8">
+        <v>4034876</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1768170</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>5803046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8">
+        <v>2489142</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1348187</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>3837329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8">
+        <v>1545734</v>
+      </c>
+      <c r="E10" s="8">
+        <v>419983</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>1965717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="10"/>
+      <c r="D11" s="8">
+        <v>8873696</v>
+      </c>
+      <c r="E11" s="8">
+        <v>9941748</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>18815444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="8">
+        <v>459606</v>
+      </c>
+      <c r="E12" s="8">
+        <v>526685</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>986291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="8">
+        <v>847053</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1007297</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>1854350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>19991</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>19991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1911244</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3132616</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>5043860</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="8">
+        <v>320057</v>
+      </c>
+      <c r="E16" s="8">
+        <v>245939</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>565996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="22" t="s">
         <v>17</v>
       </c>
+      <c r="D17" s="8">
+        <v>437989</v>
+      </c>
+      <c r="E17" s="8">
+        <v>151911</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>589900</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="8">
+        <v>4897747</v>
+      </c>
+      <c r="E18" s="8">
+        <v>4857309</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>9755056</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
@@ -699,11 +916,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
@@ -715,233 +932,233 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
       <c r="D4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
       <c r="D6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
       <c r="D8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
       <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
       <c r="D11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="19"/>
       <c r="D12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="13" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
       <c r="D15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="20"/>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
       <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
       <c r="D26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
       <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
       <c r="D28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
       <c r="D29" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
       <c r="D30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
       <c r="D31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
@@ -949,61 +1166,61 @@
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" s="17"/>
-      <c r="D33" s="13" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="17"/>
+      <c r="C34" s="16"/>
       <c r="D34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="17"/>
+      <c r="C35" s="16"/>
       <c r="D35" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" s="17"/>
+      <c r="C36" s="16"/>
       <c r="D36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="17"/>
+      <c r="C37" s="16"/>
       <c r="D37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="17"/>
+      <c r="C38" s="16"/>
       <c r="D38" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="17"/>
+      <c r="C39" s="16"/>
       <c r="D39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="17"/>
+      <c r="C40" s="16"/>
       <c r="D40" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" s="17"/>
+      <c r="C41" s="16"/>
       <c r="D41" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
@@ -1011,61 +1228,61 @@
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C43" s="17"/>
-      <c r="D43" s="13" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="17"/>
+      <c r="C44" s="16"/>
       <c r="D44" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C45" s="17"/>
+      <c r="C45" s="16"/>
       <c r="D45" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="17"/>
+      <c r="C46" s="16"/>
       <c r="D46" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="17"/>
+      <c r="C47" s="16"/>
       <c r="D47" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="17"/>
+      <c r="C48" s="16"/>
       <c r="D48" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="17"/>
+      <c r="C49" s="16"/>
       <c r="D49" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
       <c r="D50" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="17"/>
+      <c r="C51" s="16"/>
       <c r="D51" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
@@ -1073,127 +1290,127 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="17"/>
-      <c r="D53" s="13" t="s">
+      <c r="C53" s="16"/>
+      <c r="D53" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="17"/>
+      <c r="C54" s="16"/>
       <c r="D54" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="17"/>
+      <c r="C55" s="16"/>
       <c r="D55" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="17"/>
+      <c r="C56" s="16"/>
       <c r="D56" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C57" s="17"/>
+      <c r="C57" s="16"/>
       <c r="D57" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C58" s="17"/>
+      <c r="C58" s="16"/>
       <c r="D58" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C59" s="17"/>
+      <c r="C59" s="16"/>
       <c r="D59" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C60" s="17"/>
+      <c r="C60" s="16"/>
       <c r="D60" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="17"/>
+      <c r="C61" s="16"/>
       <c r="D61" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="18"/>
+      <c r="C62" s="17"/>
       <c r="D62" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="13" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
       <c r="D64" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
       <c r="D65" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
       <c r="D66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
       <c r="D67" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
       <c r="D68" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
       <c r="D69" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
       <c r="D70" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
       <c r="D71" t="s">
         <v>19</v>
       </c>
@@ -1207,7 +1424,7 @@
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1260,7 +1477,7 @@
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1305,16 +1522,16 @@
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="7"/>
+      <c r="C92" s="10"/>
       <c r="D92" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D93" s="13" t="s">
+      <c r="D93" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1367,7 +1584,7 @@
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D103" s="13" t="s">
+      <c r="D103" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1420,7 +1637,7 @@
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D113" s="13" t="s">
+      <c r="D113" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1473,7 +1690,7 @@
       </c>
     </row>
     <row r="123" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D123" s="13" t="s">
+      <c r="D123" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1526,7 +1743,7 @@
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D133" s="13" t="s">
+      <c r="D133" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1579,7 +1796,7 @@
       </c>
     </row>
     <row r="143" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D143" s="13" t="s">
+      <c r="D143" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1656,11 +1873,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" t="s">
         <v>18</v>
       </c>
@@ -1672,11 +1889,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" t="s">
         <v>21</v>
       </c>
@@ -1693,10 +1910,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="13"/>
       <c r="D4" t="s">
         <v>21</v>
       </c>
@@ -1733,10 +1950,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="14"/>
       <c r="D8" t="s">
         <v>21</v>
       </c>
@@ -1763,10 +1980,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="10"/>
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -1822,12 +2039,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="13" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1837,17 +2054,17 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1857,7 +2074,7 @@
       <c r="C20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1867,7 +2084,7 @@
       <c r="C21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1877,17 +2094,17 @@
       <c r="C22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1897,7 +2114,7 @@
       <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1907,17 +2124,17 @@
       <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="13" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1927,7 +2144,7 @@
       <c r="C27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1937,7 +2154,7 @@
       <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1947,7 +2164,7 @@
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1957,7 +2174,7 @@
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1967,16 +2184,16 @@
       <c r="C31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" t="s">
         <v>22</v>
       </c>
@@ -1993,10 +2210,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="13"/>
       <c r="D34" t="s">
         <v>22</v>
       </c>
@@ -2033,10 +2250,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="14"/>
       <c r="D38" t="s">
         <v>22</v>
       </c>
@@ -2063,10 +2280,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="10"/>
       <c r="D41" t="s">
         <v>22</v>
       </c>
@@ -2122,11 +2339,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
       <c r="D47" t="s">
         <v>23</v>
       </c>
@@ -2143,10 +2360,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="13"/>
       <c r="D49" t="s">
         <v>23</v>
       </c>
@@ -2183,10 +2400,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="10"/>
+      <c r="C53" s="14"/>
       <c r="D53" t="s">
         <v>23</v>
       </c>
@@ -2213,10 +2430,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="7"/>
+      <c r="C56" s="10"/>
       <c r="D56" t="s">
         <v>23</v>
       </c>
@@ -2272,11 +2489,11 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
       <c r="D62" t="s">
         <v>24</v>
       </c>
@@ -2293,10 +2510,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="9"/>
+      <c r="C64" s="13"/>
       <c r="D64" t="s">
         <v>24</v>
       </c>
@@ -2333,10 +2550,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="10"/>
+      <c r="C68" s="14"/>
       <c r="D68" t="s">
         <v>24</v>
       </c>
@@ -2363,10 +2580,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="7"/>
+      <c r="C71" s="10"/>
       <c r="D71" t="s">
         <v>24</v>
       </c>
@@ -2422,11 +2639,11 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
       <c r="D77" t="s">
         <v>25</v>
       </c>
@@ -2443,10 +2660,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="9"/>
+      <c r="C79" s="13"/>
       <c r="D79" t="s">
         <v>25</v>
       </c>
@@ -2483,10 +2700,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="10"/>
+      <c r="C83" s="14"/>
       <c r="D83" t="s">
         <v>25</v>
       </c>
@@ -2513,10 +2730,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="7"/>
+      <c r="C86" s="10"/>
       <c r="D86" t="s">
         <v>25</v>
       </c>
@@ -2572,11 +2789,11 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
       <c r="D92" t="s">
         <v>26</v>
       </c>
@@ -2593,10 +2810,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C94" s="9"/>
+      <c r="C94" s="13"/>
       <c r="D94" t="s">
         <v>26</v>
       </c>
@@ -2633,10 +2850,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="10"/>
+      <c r="C98" s="14"/>
       <c r="D98" t="s">
         <v>26</v>
       </c>
@@ -2663,10 +2880,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="7"/>
+      <c r="C101" s="10"/>
       <c r="D101" t="s">
         <v>26</v>
       </c>
@@ -2722,11 +2939,11 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="15"/>
       <c r="D107" t="s">
         <v>27</v>
       </c>
@@ -2743,10 +2960,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C109" s="9"/>
+      <c r="C109" s="13"/>
       <c r="D109" t="s">
         <v>27</v>
       </c>
@@ -2783,10 +3000,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="5"/>
-      <c r="B113" s="10" t="s">
+      <c r="B113" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C113" s="10"/>
+      <c r="C113" s="14"/>
       <c r="D113" t="s">
         <v>27</v>
       </c>
@@ -2813,10 +3030,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="5"/>
-      <c r="B116" s="7" t="s">
+      <c r="B116" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C116" s="7"/>
+      <c r="C116" s="10"/>
       <c r="D116" t="s">
         <v>27</v>
       </c>
@@ -2872,11 +3089,11 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="11" t="s">
+      <c r="A122" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="15"/>
       <c r="D122" t="s">
         <v>28</v>
       </c>
@@ -2893,10 +3110,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="5"/>
-      <c r="B124" s="9" t="s">
+      <c r="B124" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C124" s="9"/>
+      <c r="C124" s="13"/>
       <c r="D124" t="s">
         <v>28</v>
       </c>
@@ -2933,10 +3150,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="5"/>
-      <c r="B128" s="10" t="s">
+      <c r="B128" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C128" s="10"/>
+      <c r="C128" s="14"/>
       <c r="D128" t="s">
         <v>28</v>
       </c>
@@ -2963,10 +3180,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
-      <c r="B131" s="7" t="s">
+      <c r="B131" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C131" s="7"/>
+      <c r="C131" s="10"/>
       <c r="D131" t="s">
         <v>28</v>
       </c>
@@ -3022,11 +3239,11 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
+      <c r="A137" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B137" s="11"/>
-      <c r="C137" s="11"/>
+      <c r="B137" s="15"/>
+      <c r="C137" s="15"/>
       <c r="D137" t="s">
         <v>19</v>
       </c>
@@ -3043,10 +3260,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
-      <c r="B139" s="9" t="s">
+      <c r="B139" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C139" s="9"/>
+      <c r="C139" s="13"/>
       <c r="D139" t="s">
         <v>19</v>
       </c>
@@ -3083,10 +3300,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="5"/>
-      <c r="B143" s="10" t="s">
+      <c r="B143" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C143" s="10"/>
+      <c r="C143" s="14"/>
       <c r="D143" t="s">
         <v>19</v>
       </c>
@@ -3113,10 +3330,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
-      <c r="B146" s="7" t="s">
+      <c r="B146" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C146" s="7"/>
+      <c r="C146" s="10"/>
       <c r="D146" t="s">
         <v>19</v>
       </c>
@@ -3179,11 +3396,6 @@
     <mergeCell ref="B131:C131"/>
     <mergeCell ref="A137:C137"/>
     <mergeCell ref="B138:C138"/>
-    <mergeCell ref="A107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B116:C116"/>
     <mergeCell ref="A122:C122"/>
     <mergeCell ref="B86:C86"/>
     <mergeCell ref="A92:C92"/>
@@ -3191,11 +3403,11 @@
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="B98:C98"/>
     <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="A107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B116:C116"/>
     <mergeCell ref="B83:C83"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="B53:C53"/>
@@ -3203,11 +3415,11 @@
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -3215,12 +3427,17 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3244,25 +3461,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" t="s">
         <v>21</v>
       </c>
@@ -3295,11 +3512,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
@@ -3310,10 +3527,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -3338,10 +3555,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -3359,10 +3576,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
@@ -3401,13 +3618,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="D1:M1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3417,8 +3634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,25 +3648,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" t="s">
         <v>21</v>
       </c>
@@ -3482,11 +3699,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
@@ -3497,10 +3714,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -3525,10 +3742,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -3546,10 +3763,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>

</xml_diff>